<commit_message>
Added ML_readme and screenshots with updates on ML script & ML_output.csv.
</commit_message>
<xml_diff>
--- a/Machine_Learning/DB_DataInfo.xlsx
+++ b/Machine_Learning/DB_DataInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinuthaphani/Documents/Vinutha_GitHUB/Final_Project/final_project/Machine_Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010E1244-4566-D445-A7FE-A5DF6F0945AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1F0F79-DF63-C140-8590-F39A220110B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20440" xr2:uid="{680B78EA-BF2A-F248-BB59-BC32D6BD87FD}"/>
+    <workbookView xWindow="37940" yWindow="460" windowWidth="35840" windowHeight="20440" xr2:uid="{680B78EA-BF2A-F248-BB59-BC32D6BD87FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,10 +424,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -448,20 +454,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,10 +810,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="44" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="18">
         <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -827,8 +827,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
@@ -840,10 +840,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="15">
         <v>6000</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -857,8 +857,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
@@ -870,8 +870,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -883,8 +883,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
@@ -896,10 +896,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="18">
         <v>1508</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -913,8 +913,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
@@ -926,8 +926,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
@@ -939,10 +939,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="15">
         <v>3068</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -956,8 +956,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
@@ -969,8 +969,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
@@ -982,10 +982,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="18">
         <v>1144</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -999,8 +999,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1012,8 +1012,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="5" t="s">
         <v>30</v>
       </c>
@@ -1025,10 +1025,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="15">
         <v>2132</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1042,8 +1042,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1055,8 +1055,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1068,8 +1068,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="3" t="s">
         <v>34</v>
       </c>
@@ -1081,8 +1081,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="3" t="s">
         <v>35</v>
       </c>
@@ -1094,8 +1094,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="3" t="s">
         <v>36</v>
       </c>
@@ -1107,8 +1107,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
@@ -1120,8 +1120,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="3" t="s">
         <v>38</v>
       </c>
@@ -1133,8 +1133,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="3" t="s">
         <v>39</v>
       </c>
@@ -1146,10 +1146,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="18">
         <v>48</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1163,8 +1163,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="5" t="s">
         <v>45</v>
       </c>
@@ -1176,8 +1176,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="5" t="s">
         <v>46</v>
       </c>
@@ -1189,8 +1189,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="5" t="s">
         <v>47</v>
       </c>
@@ -1202,8 +1202,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="5" t="s">
         <v>48</v>
       </c>
@@ -1215,8 +1215,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="5" t="s">
         <v>49</v>
       </c>
@@ -1228,8 +1228,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="5" t="s">
         <v>50</v>
       </c>
@@ -1241,10 +1241,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="15">
         <v>125</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1258,8 +1258,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1271,8 +1271,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
@@ -1284,8 +1284,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="3" t="s">
         <v>9</v>
       </c>
@@ -1297,10 +1297,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="18">
         <v>3068</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1314,8 +1314,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
@@ -1327,8 +1327,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="5" t="s">
         <v>57</v>
       </c>
@@ -1340,8 +1340,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="5" t="s">
         <v>58</v>
       </c>
@@ -1353,8 +1353,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="5" t="s">
         <v>59</v>
       </c>
@@ -1366,8 +1366,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="5" t="s">
         <v>60</v>
       </c>
@@ -1379,8 +1379,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="5" t="s">
         <v>61</v>
       </c>
@@ -1392,8 +1392,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="5" t="s">
         <v>62</v>
       </c>
@@ -1405,8 +1405,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="5" t="s">
         <v>63</v>
       </c>
@@ -1418,8 +1418,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="5" t="s">
         <v>64</v>
       </c>
@@ -1431,8 +1431,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
       <c r="C47" s="5" t="s">
         <v>65</v>
       </c>
@@ -1444,8 +1444,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
       <c r="C48" s="5" t="s">
         <v>66</v>
       </c>
@@ -1457,10 +1457,10 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="13"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="3" t="s">
         <v>5</v>
       </c>
@@ -1472,8 +1472,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="14"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="16"/>
       <c r="C50" s="3" t="s">
         <v>7</v>
       </c>
@@ -1483,8 +1483,8 @@
       <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="4" t="s">
         <v>28</v>
       </c>
@@ -1495,18 +1495,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A25"/>
-    <mergeCell ref="B17:B25"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A26:A32"/>
@@ -1515,6 +1503,18 @@
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="A37:A48"/>
     <mergeCell ref="B37:B48"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A25"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>